<commit_message>
Fixing up cube analysis
</commit_message>
<xml_diff>
--- a/RedwoodPLG/Cube Analysis.xlsx
+++ b/RedwoodPLG/Cube Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grace Brockwell\OneDrive\Fourth Year\Fall Quarter\INFO 3300\Peer Learning Group Project\Redwood-Peer-Learning-Project\RedwoodPLG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="0693B4DAC125FA7DE8CAD0505C6470D26FA4837A" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{EFF61176-596D-4BE1-996C-1E0EFA3B0287}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="0693B4DAC125FA7DE8CAD0505C6470D26FA4837A" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E22FB47B-CAC1-4B4B-AEC1-EAF53E9F3D9A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="12" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2747,48 +2747,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Grace Brockwell" refreshedDate="43046.451241087962" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF7C010000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Grace Brockwell" refreshedDate="43046.466457175928" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF7C010000}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="9">
-    <cacheField name="[Dim Agent].[Agent Drill].[Last Name]" caption="Last Name" numFmtId="0" hierarchy="5" level="1">
-      <sharedItems count="29">
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Allee]" c="Allee"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Carling]" c="Carling"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Chong]" c="Chong"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Dahlen]" c="Dahlen"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Dann]" c="Dann"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Fernandez]" c="Fernandez"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Flamenbaum]" c="Flamenbaum"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Gagnon]" c="Gagnon"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Herring]" c="Herring"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Kellogg]" c="Kellogg"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Lewis]" c="Lewis"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Marcoux]" c="Marcoux"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Okindo]" c="Okindo"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Piperova]" c="Piperova"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Reed]" c="Reed"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Robinson]" c="Robinson"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Romero]" c="Romero"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Rowe]" c="Rowe"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Schutz]" c="Schutz"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Selby]" c="Selby"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Sheibani]" c="Sheibani"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Silverburg]" c="Silverburg"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Soltwedel]" c="Soltwedel"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[St-Onge]" c="St-Onge"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Taylor]" c="Taylor"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Townsend]" c="Townsend"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Voss]" c="Voss"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Weber]" c="Weber"/>
-        <s v="[Dim Agent].[Agent Drill].[Last Name].&amp;[Williams]" c="Williams"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Dim Agent].[Agent Drill].[Agent SK]" caption="Agent SK" numFmtId="0" hierarchy="5" level="2">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Dim Agent].[Agent Drill].[Agent SK].[Last Name]" caption="Last Name" propertyName="Last Name" numFmtId="0" hierarchy="5" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
+  <cacheFields count="7">
     <cacheField name="[Dim Property].[Property City Hierarchy].[City]" caption="City" numFmtId="0" hierarchy="12" level="1">
       <sharedItems count="9">
         <s v="[Dim Property].[Property City Hierarchy].[City].&amp;[Arcata]" c="Arcata"/>
@@ -2815,6 +2776,39 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Measures].[Fact Contacts Count]" caption="Fact Contacts Count" numFmtId="0" hierarchy="15" level="32767"/>
+    <cacheField name="[Dim Agent].[Last Name].[Last Name]" caption="Last Name" numFmtId="0" hierarchy="7" level="1">
+      <sharedItems count="29">
+        <s v="[Dim Agent].[Last Name].&amp;[Allee]" c="Allee"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Carling]" c="Carling"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Chong]" c="Chong"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Dahlen]" c="Dahlen"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Dann]" c="Dann"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Fernandez]" c="Fernandez"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Flamenbaum]" c="Flamenbaum"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Gagnon]" c="Gagnon"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Herring]" c="Herring"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Kellogg]" c="Kellogg"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Lewis]" c="Lewis"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Marcoux]" c="Marcoux"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Okindo]" c="Okindo"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Piperova]" c="Piperova"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Reed]" c="Reed"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Robinson]" c="Robinson"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Romero]" c="Romero"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Rowe]" c="Rowe"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Schutz]" c="Schutz"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Selby]" c="Selby"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Sheibani]" c="Sheibani"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Silverburg]" c="Silverburg"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Soltwedel]" c="Soltwedel"/>
+        <s v="[Dim Agent].[Last Name].&amp;[St-Onge]" c="St-Onge"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Taylor]" c="Taylor"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Townsend]" c="Townsend"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Voss]" c="Voss"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Weber]" c="Weber"/>
+        <s v="[Dim Agent].[Last Name].&amp;[Williams]" c="Williams"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
   <cacheHierarchies count="20">
     <cacheHierarchy uniqueName="[Date].[Date]" caption="Date" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Date].[Date].[All]" allUniqueName="[Date].[Date].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
@@ -2822,15 +2816,14 @@
     <cacheHierarchy uniqueName="[Date].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Date].[Month].[All]" allUniqueName="[Date].[Month].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Date].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Date].[Quarter].[All]" allUniqueName="[Date].[Quarter].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Date].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Date].[Year].[All]" allUniqueName="[Date].[Year].[All]" dimensionUniqueName="[Date]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Agent].[Agent Drill]" caption="Agent Drill" defaultMemberUniqueName="[Dim Agent].[Agent Drill].[All]" allUniqueName="[Dim Agent].[Agent Drill].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="3" unbalanced="0">
-      <fieldsUsage count="3">
+    <cacheHierarchy uniqueName="[Dim Agent].[Agent Drill]" caption="Agent Drill" defaultMemberUniqueName="[Dim Agent].[Agent Drill].[All]" allUniqueName="[Dim Agent].[Agent Drill].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="3" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Agent].[Agent SK]" caption="Agent SK" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Agent].[Agent SK].[All]" allUniqueName="[Dim Agent].[Agent SK].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Dim Agent].[Last Name]" caption="Last Name" attribute="1" defaultMemberUniqueName="[Dim Agent].[Last Name].[All]" allUniqueName="[Dim Agent].[Last Name].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-        <fieldUsage x="1"/>
+        <fieldUsage x="6"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Dim Agent].[Agent SK]" caption="Agent SK" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Agent].[Agent SK].[All]" allUniqueName="[Dim Agent].[Agent SK].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Dim Agent].[Last Name]" caption="Last Name" attribute="1" defaultMemberUniqueName="[Dim Agent].[Last Name].[All]" allUniqueName="[Dim Agent].[Last Name].[All]" dimensionUniqueName="[Dim Agent]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Dim Listing].[Asking Price]" caption="Asking Price" attribute="1" defaultMemberUniqueName="[Dim Listing].[Asking Price].[All]" allUniqueName="[Dim Listing].[Asking Price].[All]" dimensionUniqueName="[Dim Listing]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Dim Listing].[Listing Hierarchy]" caption="Listing Hierarchy" defaultMemberUniqueName="[Dim Listing].[Listing Hierarchy].[All]" allUniqueName="[Dim Listing].[Listing Hierarchy].[All]" dimensionUniqueName="[Dim Listing]" displayFolder="" count="2" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Dim Listing].[Listing SK]" caption="Listing SK" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Listing].[Listing SK].[All]" allUniqueName="[Dim Listing].[Listing SK].[All]" dimensionUniqueName="[Dim Listing]" displayFolder="" count="0" unbalanced="0"/>
@@ -2838,16 +2831,16 @@
     <cacheHierarchy uniqueName="[Dim Property].[Property City Hierarchy]" caption="Property City Hierarchy" defaultMemberUniqueName="[Dim Property].[Property City Hierarchy].[All]" allUniqueName="[Dim Property].[Property City Hierarchy].[All]" dimensionUniqueName="[Dim Property]" displayFolder="" count="4" unbalanced="0">
       <fieldsUsage count="4">
         <fieldUsage x="-1"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-        <fieldUsage x="5"/>
+        <fieldUsage x="0"/>
+        <fieldUsage x="1"/>
+        <fieldUsage x="2"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Dim Property].[Property SK]" caption="Property SK" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Dim Property].[Property SK].[All]" allUniqueName="[Dim Property].[Property SK].[All]" dimensionUniqueName="[Dim Property]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Dim Property].[Zipcode]" caption="Zipcode" attribute="1" defaultMemberUniqueName="[Dim Property].[Zipcode].[All]" allUniqueName="[Dim Property].[Zipcode].[All]" dimensionUniqueName="[Dim Property]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[Fact Contacts Count]" caption="Fact Contacts Count" measure="1" displayFolder="" measureGroup="Fact Contacts" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="8"/>
+        <fieldUsage x="5"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Average Contacts Per Listing]" caption="Average Contacts Per Listing" measure="1" displayFolder="" measureGroup="Fact Contacts" count="0"/>
@@ -2881,49 +2874,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A1:B173" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
-      <items count="30">
-        <item c="1" x="0"/>
-        <item c="1" x="1"/>
-        <item c="1" x="2"/>
-        <item c="1" x="3"/>
-        <item c="1" x="4"/>
-        <item c="1" x="5"/>
-        <item c="1" x="6"/>
-        <item c="1" x="7"/>
-        <item c="1" x="8"/>
-        <item c="1" x="9"/>
-        <item c="1" x="10"/>
-        <item c="1" x="11"/>
-        <item c="1" x="12"/>
-        <item c="1" x="13"/>
-        <item c="1" x="14"/>
-        <item c="1" x="15"/>
-        <item c="1" x="16"/>
-        <item c="1" x="17"/>
-        <item c="1" x="18"/>
-        <item c="1" x="19"/>
-        <item c="1" x="20"/>
-        <item c="1" x="21"/>
-        <item c="1" x="22"/>
-        <item c="1" x="23"/>
-        <item c="1" x="24"/>
-        <item c="1" x="25"/>
-        <item c="1" x="26"/>
-        <item c="1" x="27"/>
-        <item c="1" x="28"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
-      <items count="1">
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" dataSourceSort="1" showPropTip="1"/>
+  <pivotFields count="7">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
       <items count="10">
         <item c="1" x="0"/>
@@ -2951,10 +2904,44 @@
     <pivotField showAll="0" dataSourceSort="1" showPropTip="1"/>
     <pivotField showAll="0" dataSourceSort="1" showPropTip="1"/>
     <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="30">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="2">
-    <field x="3"/>
     <field x="0"/>
+    <field x="6"/>
   </rowFields>
   <rowItems count="172">
     <i>
@@ -3478,7 +3465,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField fld="8" baseField="0" baseItem="0"/>
+    <dataField fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="2" series="1">
@@ -3497,11 +3484,7 @@
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
-    <pivotHierarchy>
-      <mps count="1">
-        <mp field="2"/>
-      </mps>
-    </pivotHierarchy>
+    <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3510,8 +3493,8 @@
     <pivotHierarchy/>
     <pivotHierarchy>
       <mps count="2">
-        <mp field="6"/>
-        <mp field="7"/>
+        <mp field="3"/>
+        <mp field="4"/>
       </mps>
     </pivotHierarchy>
     <pivotHierarchy/>
@@ -3525,7 +3508,7 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
     <rowHierarchyUsage hierarchyUsage="12"/>
-    <rowHierarchyUsage hierarchyUsage="5"/>
+    <rowHierarchyUsage hierarchyUsage="7"/>
   </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3838,7 +3821,7 @@
   <dimension ref="A1:Q173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>